<commit_message>
Separation of the main page and the mathematical details.
</commit_message>
<xml_diff>
--- a/posts/vcvs-finite-gbw/vcvs-example-01.xlsx
+++ b/posts/vcvs-finite-gbw/vcvs-example-01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\hadrien\Electronique\2025-New-Site\f4inx.github.io\posts\vcvs-finite-gbw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\hadrien\CLOUD\Electronique\New site\f4inx.github.io\posts\vcvs-finite-gbw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476E728D-98AC-4EA6-BE35-755C78EE699A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26E547D-E5C3-49C0-A621-64CB43467346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{EE353CA1-25B1-4D54-82AA-D5A9EF3ADA65}"/>
   </bookViews>
@@ -36,11 +36,11 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="7">
+  <futureMetadata name="XLRICHVALUE" count="6">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -83,15 +83,8 @@
         </ext>
       </extLst>
     </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="6"/>
-        </ext>
-      </extLst>
-    </bk>
   </futureMetadata>
-  <valueMetadata count="7">
+  <valueMetadata count="6">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -109,19 +102,13 @@
     </bk>
     <bk>
       <rc t="1" v="5"/>
-    </bk>
-    <bk>
-      <rc t="1" v="6"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
-  <si>
-    <t>Q</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>s</t>
   </si>
@@ -168,9 +155,6 @@
     <t>Components values</t>
   </si>
   <si>
-    <t>Hypothesis check</t>
-  </si>
-  <si>
     <t>LM324, TI datasheet.</t>
   </si>
   <si>
@@ -178,6 +162,30 @@
   </si>
   <si>
     <t>Hypothesis used in calculations. OK.</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>Validity conditions</t>
+  </si>
+  <si>
+    <t>&gt;&gt; 1</t>
+  </si>
+  <si>
+    <t>fp</t>
+  </si>
+  <si>
+    <t>fp/BW</t>
+  </si>
+  <si>
+    <t>Frequency of the parasitic low-pass (pole)</t>
+  </si>
+  <si>
+    <t>Yes, this is a little higher than GBW.</t>
+  </si>
+  <si>
+    <t>TODO: Simplify these equations.</t>
   </si>
 </sst>
 </file>
@@ -238,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -249,6 +257,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -309,7 +323,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="7">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -334,10 +348,6 @@
     <v>5</v>
     <v>5</v>
   </rv>
-  <rv s="0">
-    <v>6</v>
-    <v>5</v>
-  </rv>
 </rvData>
 </file>
 
@@ -358,7 +368,6 @@
   <rel r:id="rId4"/>
   <rel r:id="rId5"/>
   <rel r:id="rId6"/>
-  <rel r:id="rId7"/>
 </richValueRels>
 </file>
 
@@ -625,7 +634,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B74BCFF-1F51-417A-8DE0-0ACC4826765C}">
-  <dimension ref="B2:H33"/>
+  <dimension ref="B2:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -638,202 +647,288 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3">
         <v>330</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>1.2</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
         <f>C3*1000</f>
         <v>40000</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B10" t="e" vm="1">
-        <v>#VALUE!</v>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
       <c r="C10" s="1">
-        <f>1/(2*PI()*C9)</f>
-        <v>3.9788735772973834E-6</v>
+        <f>C4*1000</f>
+        <v>10000</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <f>C5*0.000000000001</f>
         <v>3.3E-10</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B12" t="e" vm="2">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <f>C6*1000000</f>
+        <v>1200000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B15" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C15" s="5">
+        <f>(1/(PI()*C10*C11))*(1-C10/C12)/(1+(2*C9^2)/(C10*C12))</f>
+        <v>75516.101387302828</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B16" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C16" s="1">
+        <f>C10/(4*PI()*C9^2*C11)</f>
+        <v>1507.1490823096151</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="18" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C19" s="1">
+        <f>1/(2*PI()*C9)</f>
+        <v>3.9788735772973834E-6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B20" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C20" s="1">
         <f>C6*1000000*2*PI()</f>
         <v>7539822.3686155034</v>
       </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B14" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B15" t="e" vm="3">
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B21" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="C15" s="5">
-        <f>2*C4*C10/C11*(1-1/(C4*C12*C10))/(1+(2*C4)/(C12*C10))</f>
-        <v>75516.101387302813</v>
-      </c>
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B16" t="e" vm="4">
+      <c r="C21" s="1">
+        <f>(C16*C15*C11^2)/(C19^2*C20)</f>
+        <v>1.0383463940754141E-7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1">
+        <f>1/(2*PI()*C21)</f>
+        <v>1532773.1092436968</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="3">
+        <f>C22/1000000</f>
+        <v>1.5327731092436967</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="6">
+        <f>C22/C10</f>
+        <v>153.27731092436969</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
-      <c r="C16" s="1">
-        <f>C10/(2*C4*C11)</f>
+      <c r="C28" s="6">
+        <f>(2*C16)/((2*C16+C15)/(2*PI()*C12))</f>
+        <v>289407.32323978696</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C37" s="1"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B44" s="1">
+        <v>75516.101387302828</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B45" s="1">
         <v>1507.1490823096149</v>
       </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="18" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B19" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C19" s="1">
-        <f>(C16*C15*C11^2)/(C10^2*C12)</f>
-        <v>1.0383463940754137E-7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" t="e" vm="6">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C20" s="6">
-        <f>(C10^2)/(C10*C19/C4)</f>
-        <v>153.27731092436974</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" t="e" vm="7">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C21" s="6">
-        <f>(2*C16)/((2*C16+C15)/C12)</f>
-        <v>289407.32323978696</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="D24" s="2"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C26" s="1"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.45">
-      <c r="C33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Second validity equation for details only.
</commit_message>
<xml_diff>
--- a/posts/vcvs-finite-gbw/vcvs-example-01.xlsx
+++ b/posts/vcvs-finite-gbw/vcvs-example-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\hadrien\CLOUD\Electronique\New site\f4inx.github.io\posts\vcvs-finite-gbw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112A4C07-7FB9-4734-A21A-461F08BE1CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD86E583-9C03-4CE0-AD63-DBDD43E8E6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{EE353CA1-25B1-4D54-82AA-D5A9EF3ADA65}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="3">
+  <futureMetadata name="XLRICHVALUE" count="2">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -55,30 +55,20 @@
         </ext>
       </extLst>
     </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="2"/>
-        </ext>
-      </extLst>
-    </bk>
   </futureMetadata>
-  <valueMetadata count="3">
+  <valueMetadata count="2">
     <bk>
       <rc t="1" v="0"/>
     </bk>
     <bk>
       <rc t="1" v="1"/>
     </bk>
-    <bk>
-      <rc t="1" v="2"/>
-    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>f0</t>
   </si>
@@ -125,9 +115,6 @@
     <t>Hypothesis used in factorisation. OK.</t>
   </si>
   <si>
-    <t>Hypothesis used in calculations. OK.</t>
-  </si>
-  <si>
     <t>BW</t>
   </si>
   <si>
@@ -140,16 +127,10 @@
     <t>fp</t>
   </si>
   <si>
-    <t>fp/BW</t>
-  </si>
-  <si>
     <t>Frequency of the parasitic low-pass (pole)</t>
   </si>
   <si>
     <t>Yes, this is a little higher than GBW.</t>
-  </si>
-  <si>
-    <t>TODO: Simplify these equations.</t>
   </si>
 </sst>
 </file>
@@ -210,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -229,7 +210,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -247,6 +227,55 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>536494</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14888</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3E4F5FF-51AC-1FA6-A769-99A5F164C0CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="223838" y="4162425"/>
+          <a:ext cx="536494" cy="329213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
 <rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
@@ -288,7 +317,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -297,10 +326,6 @@
     <v>1</v>
     <v>5</v>
   </rv>
-  <rv s="0">
-    <v>2</v>
-    <v>5</v>
-  </rv>
 </rvData>
 </file>
 
@@ -317,7 +342,6 @@
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
   <rel r:id="rId2"/>
-  <rel r:id="rId3"/>
 </richValueRels>
 </file>
 
@@ -584,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B74BCFF-1F51-417A-8DE0-0ACC4826765C}">
-  <dimension ref="B2:H36"/>
+  <dimension ref="B2:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -613,7 +637,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -669,7 +693,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1">
         <f>C4*1000</f>
@@ -737,25 +761,25 @@
     </row>
     <row r="18" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1">
         <f>C12*(1+(2*C9^2)/(C10*C12))/(1-C10/C12)</f>
         <v>1532773.1092436975</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="3">
         <f>C19/1000000</f>
@@ -765,7 +789,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.45">
@@ -773,66 +797,44 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="2:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="6">
+    <row r="23" spans="2:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="9"/>
+      <c r="C23" s="6">
         <f>C19/C10</f>
         <v>153.27731092436974</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="7" t="s">
+      <c r="D23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C25" s="6">
-        <f>(2*C16)/((2*C16+C15)/(2*PI()*C12))</f>
-        <v>289407.32323978696</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>15</v>
-      </c>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="C31" s="1"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B36" s="1"/>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>